<commit_message>
add splash screen and making library manager
</commit_message>
<xml_diff>
--- a/ccIDE Defines.xlsx
+++ b/ccIDE Defines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sansw\Desktop\ccIDE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B13E89DA-B80E-4831-B1C8-8A4785BCA506}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EDC02CC-8823-4B10-A2D3-A2622C3ED74C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A1762A9E-4243-4645-BD88-14F570C693A0}"/>
+    <workbookView minimized="1" xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{A1762A9E-4243-4645-BD88-14F570C693A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Function" sheetId="1" r:id="rId1"/>
@@ -2691,7 +2691,7 @@
     <t>File Access</t>
   </si>
   <si>
-    <t>https://tweaked.cc/module/term.html</t>
+    <t>Skip for other group</t>
   </si>
 </sst>
 </file>
@@ -3230,7 +3230,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3528,9 +3528,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="44" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="45" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -3885,8 +3882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1435FBCC-F7BC-474D-9F6E-055E473444AC}">
   <dimension ref="A1:M222"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D177" sqref="D177"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3945,7 +3942,7 @@
       <c r="M1" s="1"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="50" t="s">
         <v>15</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -4110,7 +4107,7 @@
       <c r="M6" s="7"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="51" t="s">
+      <c r="A7" s="6" t="s">
         <v>119</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -4950,7 +4947,7 @@
       <c r="B33" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="C33" s="108" t="s">
+      <c r="C33" s="107" t="s">
         <v>883</v>
       </c>
       <c r="D33" s="4" t="s">
@@ -4983,7 +4980,7 @@
       <c r="B34" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="C34" s="108" t="s">
+      <c r="C34" s="107" t="s">
         <v>883</v>
       </c>
       <c r="D34" s="4" t="s">
@@ -5018,7 +5015,7 @@
       <c r="B35" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="C35" s="108" t="s">
+      <c r="C35" s="107" t="s">
         <v>883</v>
       </c>
       <c r="D35" s="4" t="s">
@@ -5053,7 +5050,7 @@
       <c r="B36" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="C36" s="108" t="s">
+      <c r="C36" s="107" t="s">
         <v>883</v>
       </c>
       <c r="D36" s="4" t="s">
@@ -5088,7 +5085,7 @@
       <c r="B37" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="C37" s="108" t="s">
+      <c r="C37" s="107" t="s">
         <v>883</v>
       </c>
       <c r="D37" s="4" t="s">
@@ -5123,7 +5120,7 @@
       <c r="B38" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="C38" s="108" t="s">
+      <c r="C38" s="107" t="s">
         <v>883</v>
       </c>
       <c r="D38" s="4" t="s">
@@ -5156,7 +5153,7 @@
       <c r="B39" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="C39" s="108" t="s">
+      <c r="C39" s="107" t="s">
         <v>883</v>
       </c>
       <c r="D39" s="4" t="s">
@@ -5189,7 +5186,7 @@
       <c r="B40" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="C40" s="108" t="s">
+      <c r="C40" s="107" t="s">
         <v>883</v>
       </c>
       <c r="D40" s="4" t="s">
@@ -5224,7 +5221,7 @@
       <c r="B41" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="C41" s="108" t="s">
+      <c r="C41" s="107" t="s">
         <v>883</v>
       </c>
       <c r="D41" s="4" t="s">
@@ -5257,7 +5254,7 @@
       <c r="B42" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="C42" s="108" t="s">
+      <c r="C42" s="107" t="s">
         <v>883</v>
       </c>
       <c r="D42" s="4" t="s">
@@ -5290,7 +5287,7 @@
       <c r="B43" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="C43" s="108" t="s">
+      <c r="C43" s="107" t="s">
         <v>883</v>
       </c>
       <c r="D43" s="4" t="s">
@@ -5323,7 +5320,7 @@
       <c r="B44" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="C44" s="108" t="s">
+      <c r="C44" s="107" t="s">
         <v>883</v>
       </c>
       <c r="D44" s="4" t="s">
@@ -5358,7 +5355,7 @@
       <c r="B45" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="C45" s="108" t="s">
+      <c r="C45" s="107" t="s">
         <v>883</v>
       </c>
       <c r="D45" s="4" t="s">
@@ -5393,7 +5390,7 @@
       <c r="B46" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="C46" s="108" t="s">
+      <c r="C46" s="107" t="s">
         <v>883</v>
       </c>
       <c r="D46" s="4" t="s">
@@ -5428,7 +5425,7 @@
       <c r="B47" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="C47" s="108" t="s">
+      <c r="C47" s="107" t="s">
         <v>883</v>
       </c>
       <c r="D47" s="4" t="s">
@@ -5463,7 +5460,7 @@
       <c r="B48" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="C48" s="108" t="s">
+      <c r="C48" s="107" t="s">
         <v>883</v>
       </c>
       <c r="D48" s="4" t="s">
@@ -5498,7 +5495,7 @@
       <c r="B49" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="C49" s="108" t="s">
+      <c r="C49" s="107" t="s">
         <v>883</v>
       </c>
       <c r="D49" s="4" t="s">
@@ -5533,7 +5530,7 @@
       <c r="B50" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="C50" s="108" t="s">
+      <c r="C50" s="107" t="s">
         <v>883</v>
       </c>
       <c r="D50" s="4" t="s">
@@ -5568,7 +5565,7 @@
       <c r="B51" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="C51" s="108" t="s">
+      <c r="C51" s="107" t="s">
         <v>883</v>
       </c>
       <c r="D51" s="4" t="s">
@@ -5603,7 +5600,7 @@
       <c r="B52" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="C52" s="108" t="s">
+      <c r="C52" s="107" t="s">
         <v>883</v>
       </c>
       <c r="D52" s="4" t="s">
@@ -8258,7 +8255,7 @@
       <c r="B133" s="4" t="s">
         <v>710</v>
       </c>
-      <c r="C133" s="105" t="s">
+      <c r="C133" s="104" t="s">
         <v>710</v>
       </c>
       <c r="D133" s="4"/>
@@ -8289,7 +8286,7 @@
       <c r="B134" s="4" t="s">
         <v>710</v>
       </c>
-      <c r="C134" s="105" t="s">
+      <c r="C134" s="104" t="s">
         <v>710</v>
       </c>
       <c r="D134" s="4" t="s">
@@ -8322,7 +8319,7 @@
       <c r="B135" s="4" t="s">
         <v>710</v>
       </c>
-      <c r="C135" s="105" t="s">
+      <c r="C135" s="104" t="s">
         <v>710</v>
       </c>
       <c r="D135" s="4" t="s">
@@ -8355,7 +8352,7 @@
       <c r="B136" s="4" t="s">
         <v>710</v>
       </c>
-      <c r="C136" s="105" t="s">
+      <c r="C136" s="104" t="s">
         <v>710</v>
       </c>
       <c r="D136" s="4" t="s">
@@ -8388,7 +8385,7 @@
       <c r="B137" s="4" t="s">
         <v>710</v>
       </c>
-      <c r="C137" s="105" t="s">
+      <c r="C137" s="104" t="s">
         <v>710</v>
       </c>
       <c r="D137" s="4" t="s">
@@ -8423,7 +8420,7 @@
       <c r="B138" s="4" t="s">
         <v>710</v>
       </c>
-      <c r="C138" s="105" t="s">
+      <c r="C138" s="104" t="s">
         <v>710</v>
       </c>
       <c r="D138" s="4" t="s">
@@ -8456,7 +8453,7 @@
       <c r="B139" s="4" t="s">
         <v>710</v>
       </c>
-      <c r="C139" s="105" t="s">
+      <c r="C139" s="104" t="s">
         <v>710</v>
       </c>
       <c r="D139" s="4" t="s">
@@ -8489,7 +8486,7 @@
       <c r="B140" s="4" t="s">
         <v>710</v>
       </c>
-      <c r="C140" s="105" t="s">
+      <c r="C140" s="104" t="s">
         <v>710</v>
       </c>
       <c r="D140" s="4" t="s">
@@ -8522,7 +8519,7 @@
       <c r="B141" s="4" t="s">
         <v>710</v>
       </c>
-      <c r="C141" s="105" t="s">
+      <c r="C141" s="104" t="s">
         <v>710</v>
       </c>
       <c r="D141" s="4" t="s">
@@ -8555,7 +8552,7 @@
       <c r="B142" s="4" t="s">
         <v>710</v>
       </c>
-      <c r="C142" s="105" t="s">
+      <c r="C142" s="104" t="s">
         <v>710</v>
       </c>
       <c r="D142" s="1" t="s">
@@ -8587,7 +8584,7 @@
       <c r="B143" s="4" t="s">
         <v>710</v>
       </c>
-      <c r="C143" s="105" t="s">
+      <c r="C143" s="104" t="s">
         <v>710</v>
       </c>
       <c r="D143" s="4" t="s">
@@ -8619,7 +8616,7 @@
       <c r="B144" s="4" t="s">
         <v>761</v>
       </c>
-      <c r="C144" s="109" t="s">
+      <c r="C144" s="108" t="s">
         <v>759</v>
       </c>
       <c r="D144" s="8" t="s">
@@ -8651,7 +8648,7 @@
       <c r="B145" s="4" t="s">
         <v>761</v>
       </c>
-      <c r="C145" s="109" t="s">
+      <c r="C145" s="108" t="s">
         <v>759</v>
       </c>
       <c r="D145" s="1" t="s">
@@ -8683,7 +8680,7 @@
       <c r="B146" s="4" t="s">
         <v>761</v>
       </c>
-      <c r="C146" s="109" t="s">
+      <c r="C146" s="108" t="s">
         <v>759</v>
       </c>
       <c r="D146" s="8" t="s">
@@ -8717,7 +8714,7 @@
       <c r="B147" s="4" t="s">
         <v>761</v>
       </c>
-      <c r="C147" s="109" t="s">
+      <c r="C147" s="108" t="s">
         <v>759</v>
       </c>
       <c r="D147" s="8" t="s">
@@ -8749,7 +8746,7 @@
       <c r="B148" s="4" t="s">
         <v>761</v>
       </c>
-      <c r="C148" s="109" t="s">
+      <c r="C148" s="108" t="s">
         <v>759</v>
       </c>
       <c r="D148" s="8" t="s">
@@ -8781,7 +8778,7 @@
       <c r="B149" s="4" t="s">
         <v>761</v>
       </c>
-      <c r="C149" s="109" t="s">
+      <c r="C149" s="108" t="s">
         <v>759</v>
       </c>
       <c r="D149" s="8" t="s">
@@ -8813,7 +8810,7 @@
       <c r="B150" s="4" t="s">
         <v>761</v>
       </c>
-      <c r="C150" s="109" t="s">
+      <c r="C150" s="108" t="s">
         <v>759</v>
       </c>
       <c r="D150" s="8"/>
@@ -8843,7 +8840,7 @@
       <c r="B151" s="4" t="s">
         <v>761</v>
       </c>
-      <c r="C151" s="109" t="s">
+      <c r="C151" s="108" t="s">
         <v>759</v>
       </c>
       <c r="D151" s="8"/>
@@ -8873,7 +8870,7 @@
       <c r="B152" s="4" t="s">
         <v>761</v>
       </c>
-      <c r="C152" s="109" t="s">
+      <c r="C152" s="108" t="s">
         <v>759</v>
       </c>
       <c r="D152" s="8" t="s">
@@ -8905,7 +8902,7 @@
       <c r="B153" s="4" t="s">
         <v>761</v>
       </c>
-      <c r="C153" s="109" t="s">
+      <c r="C153" s="108" t="s">
         <v>759</v>
       </c>
       <c r="D153" s="8" t="s">
@@ -9578,7 +9575,7 @@
       <c r="A175" s="6"/>
       <c r="B175" s="4"/>
       <c r="C175" s="4"/>
-      <c r="D175" s="103" t="s">
+      <c r="D175" s="1" t="s">
         <v>884</v>
       </c>
       <c r="E175" s="4"/>
@@ -10229,10 +10226,9 @@
     <hyperlink ref="L170" r:id="rId166" location="v:aliases" xr:uid="{5949CD3E-E537-45AC-8A03-0C0D80297B6B}"/>
     <hyperlink ref="L171" r:id="rId167" location="v:openTab" xr:uid="{07FB9824-AB1F-4082-A7C2-DA8905FBA769}"/>
     <hyperlink ref="L172" r:id="rId168" location="v:switchTab" xr:uid="{796DAB75-E0D0-4CC9-954B-C7BACC6C5F9F}"/>
-    <hyperlink ref="D175" r:id="rId169" xr:uid="{CA6C5100-A5B6-409F-97C3-EF7B16895043}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId170"/>
+  <pageSetup orientation="portrait" r:id="rId169"/>
 </worksheet>
 </file>
 
@@ -10240,7 +10236,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{381D1F79-32D5-434E-9D3A-C31E8762B8B9}">
   <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -11075,7 +11071,7 @@
       <c r="B13" s="1" t="s">
         <v>711</v>
       </c>
-      <c r="C13" s="104">
+      <c r="C13" s="103">
         <v>10</v>
       </c>
       <c r="E13" s="1"/>
@@ -11099,7 +11095,7 @@
       <c r="B14" s="1" t="s">
         <v>758</v>
       </c>
-      <c r="C14" s="106">
+      <c r="C14" s="105">
         <v>144</v>
       </c>
       <c r="E14" s="1"/>
@@ -11123,7 +11119,7 @@
       <c r="B15" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="C15" s="107">
+      <c r="C15" s="106">
         <v>70</v>
       </c>
       <c r="E15" s="1"/>

</xml_diff>

<commit_message>
added new CCTurtle library (not not finish yet)
</commit_message>
<xml_diff>
--- a/ccIDE Defines.xlsx
+++ b/ccIDE Defines.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sansw\Desktop\ccIDE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EDC02CC-8823-4B10-A2D3-A2622C3ED74C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67186968-CEAD-416D-BB3E-7CE200CB62A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{A1762A9E-4243-4645-BD88-14F570C693A0}"/>
+    <workbookView xWindow="4260" yWindow="1905" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{A1762A9E-4243-4645-BD88-14F570C693A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Function" sheetId="1" r:id="rId1"/>
     <sheet name="External Func" sheetId="4" r:id="rId2"/>
-    <sheet name="Group" sheetId="2" r:id="rId3"/>
-    <sheet name="Colours" sheetId="3" r:id="rId4"/>
+    <sheet name="Value Type" sheetId="5" r:id="rId3"/>
+    <sheet name="Group" sheetId="2" r:id="rId4"/>
+    <sheet name="Colours" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1705" uniqueCount="885">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1729" uniqueCount="901">
   <si>
     <t>Name</t>
   </si>
@@ -2692,6 +2693,54 @@
   </si>
   <si>
     <t>Skip for other group</t>
+  </si>
+  <si>
+    <t>extractMultipleReturn</t>
+  </si>
+  <si>
+    <t>damp11113-library</t>
+  </si>
+  <si>
+    <t>https://chatgpt.com/share/63b1387d-8dc8-456b-91e8-2f8f0dcabcdb</t>
+  </si>
+  <si>
+    <t>Source Code</t>
+  </si>
+  <si>
+    <t>extractMultipleReturn(funcResults, index)</t>
+  </si>
+  <si>
+    <t>extract a specific return value by index</t>
+  </si>
+  <si>
+    <t>Value Type</t>
+  </si>
+  <si>
+    <t>Array</t>
+  </si>
+  <si>
+    <t>Mean in lua</t>
+  </si>
+  <si>
+    <t>Any or Real Null</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>Colour</t>
+  </si>
+  <si>
+    <t>Colour Type (not exist in lua)</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Int or Float</t>
+  </si>
+  <si>
+    <t>Multiple</t>
   </si>
 </sst>
 </file>
@@ -3230,7 +3279,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3547,6 +3596,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="46" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -3882,8 +3934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1435FBCC-F7BC-474D-9F6E-055E473444AC}">
   <dimension ref="A1:M222"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A21" sqref="A16:A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4074,7 +4126,7 @@
       <c r="M5" s="7"/>
     </row>
     <row r="6" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="50" t="s">
         <v>18</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -4107,7 +4159,7 @@
       <c r="M6" s="7"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="51" t="s">
         <v>119</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -4140,7 +4192,7 @@
       <c r="M7" s="7"/>
     </row>
     <row r="8" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="51" t="s">
         <v>125</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -10236,17 +10288,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{381D1F79-32D5-434E-9D3A-C31E8762B8B9}">
   <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="30.125" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
     <col min="4" max="4" width="22.75" customWidth="1"/>
-    <col min="5" max="5" width="18.75" customWidth="1"/>
-    <col min="6" max="6" width="22.125" customWidth="1"/>
+    <col min="5" max="5" width="40.125" customWidth="1"/>
+    <col min="6" max="6" width="34.5" customWidth="1"/>
     <col min="7" max="7" width="11.375" customWidth="1"/>
     <col min="8" max="8" width="12.875" customWidth="1"/>
+    <col min="9" max="9" width="57.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
@@ -10274,7 +10329,9 @@
       <c r="H1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="1"/>
+      <c r="I1" s="1" t="s">
+        <v>888</v>
+      </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
@@ -10306,15 +10363,31 @@
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>885</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>886</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>890</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>889</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
+      <c r="I3" s="109" t="s">
+        <v>887</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
@@ -10768,11 +10841,350 @@
       <c r="I44" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I3" r:id="rId1" xr:uid="{555E510E-19D8-4C90-8B4C-19B4B162CAC0}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5202527C-A4D9-463E-9A8C-03ED40F1A8C9}">
+  <dimension ref="A1:Q15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.25" customWidth="1"/>
+    <col min="2" max="2" width="31.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>891</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>893</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>894</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>892</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>895</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>895</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>896</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>897</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>898</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>899</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>900</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0C8232C-B27F-40EF-A66D-FBA0686F9CB5}">
   <dimension ref="A1:Q39"/>
   <sheetViews>
@@ -11585,7 +11997,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB19BC38-F9E7-4B7D-ADE1-C6476B98FD3A}">
   <dimension ref="A1:H18"/>
   <sheetViews>

</xml_diff>

<commit_message>
update 1.1.2 and add new block
added block CCRedstone and CCRednet
and CCTurtle is finished
</commit_message>
<xml_diff>
--- a/ccIDE Defines.xlsx
+++ b/ccIDE Defines.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sansw\Desktop\ccIDE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67186968-CEAD-416D-BB3E-7CE200CB62A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE7E705-944E-4F14-B2C2-162B1C2885E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4260" yWindow="1905" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{A1762A9E-4243-4645-BD88-14F570C693A0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{A1762A9E-4243-4645-BD88-14F570C693A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Function" sheetId="1" r:id="rId1"/>
     <sheet name="External Func" sheetId="4" r:id="rId2"/>
     <sheet name="Value Type" sheetId="5" r:id="rId3"/>
     <sheet name="Group" sheetId="2" r:id="rId4"/>
-    <sheet name="Colours" sheetId="3" r:id="rId5"/>
+    <sheet name="Checklist" sheetId="6" r:id="rId5"/>
+    <sheet name="Colours" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1729" uniqueCount="901">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1731" uniqueCount="902">
   <si>
     <t>Name</t>
   </si>
@@ -2741,6 +2742,9 @@
   </si>
   <si>
     <t>Multiple</t>
+  </si>
+  <si>
+    <t>Is finish</t>
   </si>
 </sst>
 </file>
@@ -3934,8 +3938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1435FBCC-F7BC-474D-9F6E-055E473444AC}">
   <dimension ref="A1:M222"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A21" sqref="A16:A21"/>
+    <sheetView topLeftCell="A154" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -10852,7 +10856,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5202527C-A4D9-463E-9A8C-03ED40F1A8C9}">
   <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -11998,6 +12002,32 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F102913-07D9-43F0-AADF-F13149DB4F36}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="27" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>901</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB19BC38-F9E7-4B7D-ADE1-C6476B98FD3A}">
   <dimension ref="A1:H18"/>
   <sheetViews>

</xml_diff>

<commit_message>
update 1.1.4 add new Settings block
add new Settings block for env settings
and merge IDE block to system for default
</commit_message>
<xml_diff>
--- a/ccIDE Defines.xlsx
+++ b/ccIDE Defines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sansw\Desktop\ccIDE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE7E705-944E-4F14-B2C2-162B1C2885E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D68855F-A651-43FC-A73C-191793FC5A63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{A1762A9E-4243-4645-BD88-14F570C693A0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A1762A9E-4243-4645-BD88-14F570C693A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Function" sheetId="1" r:id="rId1"/>
@@ -3283,7 +3283,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3603,6 +3603,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -3938,8 +3944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1435FBCC-F7BC-474D-9F6E-055E473444AC}">
   <dimension ref="A1:M222"/>
   <sheetViews>
-    <sheetView topLeftCell="A154" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4229,7 +4235,7 @@
       <c r="M8" s="7"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="50" t="s">
         <v>131</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -4262,7 +4268,7 @@
       <c r="M9" s="7"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="50" t="s">
         <v>140</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -4295,7 +4301,7 @@
       <c r="M10" s="7"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="51" t="s">
         <v>141</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -4328,7 +4334,7 @@
       <c r="M11" s="7"/>
     </row>
     <row r="12" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="51" t="s">
         <v>142</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -4361,7 +4367,7 @@
       <c r="M12" s="7"/>
     </row>
     <row r="13" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="51" t="s">
         <v>143</v>
       </c>
       <c r="B13" s="4" t="s">
@@ -4394,7 +4400,7 @@
       <c r="M13" s="7"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="51" t="s">
         <v>144</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -4427,7 +4433,7 @@
       <c r="M14" s="7"/>
     </row>
     <row r="15" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="51" t="s">
         <v>156</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -4491,7 +4497,7 @@
       <c r="M16" s="7"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="61" t="s">
+      <c r="A17" s="110" t="s">
         <v>180</v>
       </c>
       <c r="B17" s="62"/>
@@ -4515,7 +4521,7 @@
       <c r="M17" s="7"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A18" s="61" t="s">
+      <c r="A18" s="110" t="s">
         <v>181</v>
       </c>
       <c r="B18" s="62"/>
@@ -4539,7 +4545,7 @@
       <c r="M18" s="7"/>
     </row>
     <row r="19" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="65" t="s">
+      <c r="A19" s="111" t="s">
         <v>182</v>
       </c>
       <c r="B19" s="66"/>
@@ -4564,7 +4570,7 @@
       <c r="M19" s="7"/>
     </row>
     <row r="20" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="51" t="s">
         <v>193</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -4599,7 +4605,7 @@
       <c r="M20" s="7"/>
     </row>
     <row r="21" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="51" t="s">
         <v>194</v>
       </c>
       <c r="B21" s="4" t="s">
@@ -8002,7 +8008,7 @@
       <c r="M123" s="7"/>
     </row>
     <row r="124" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A124" s="6" t="s">
+      <c r="A124" s="50" t="s">
         <v>261</v>
       </c>
       <c r="B124" s="4" t="s">
@@ -8037,7 +8043,7 @@
       <c r="M124" s="7"/>
     </row>
     <row r="125" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A125" s="6" t="s">
+      <c r="A125" s="50" t="s">
         <v>400</v>
       </c>
       <c r="B125" s="4" t="s">
@@ -8072,7 +8078,7 @@
       <c r="M125" s="7"/>
     </row>
     <row r="126" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A126" s="6" t="s">
+      <c r="A126" s="50" t="s">
         <v>670</v>
       </c>
       <c r="B126" s="4" t="s">
@@ -8105,7 +8111,7 @@
       <c r="M126" s="7"/>
     </row>
     <row r="127" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A127" s="6" t="s">
+      <c r="A127" s="50" t="s">
         <v>671</v>
       </c>
       <c r="B127" s="4" t="s">
@@ -8138,7 +8144,7 @@
       <c r="M127" s="7"/>
     </row>
     <row r="128" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A128" s="6" t="s">
+      <c r="A128" s="50" t="s">
         <v>672</v>
       </c>
       <c r="B128" s="4" t="s">
@@ -8171,7 +8177,7 @@
       <c r="M128" s="7"/>
     </row>
     <row r="129" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A129" s="6" t="s">
+      <c r="A129" s="50" t="s">
         <v>673</v>
       </c>
       <c r="B129" s="4" t="s">
@@ -8204,7 +8210,7 @@
       <c r="M129" s="7"/>
     </row>
     <row r="130" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A130" s="6" t="s">
+      <c r="A130" s="50" t="s">
         <v>674</v>
       </c>
       <c r="B130" s="4" t="s">
@@ -8239,7 +8245,7 @@
       <c r="M130" s="7"/>
     </row>
     <row r="131" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A131" s="6" t="s">
+      <c r="A131" s="50" t="s">
         <v>675</v>
       </c>
       <c r="B131" s="4" t="s">
@@ -8272,7 +8278,7 @@
       <c r="M131" s="7"/>
     </row>
     <row r="132" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A132" s="6" t="s">
+      <c r="A132" s="50" t="s">
         <v>676</v>
       </c>
       <c r="B132" s="4" t="s">
@@ -8305,7 +8311,7 @@
       <c r="M132" s="7"/>
     </row>
     <row r="133" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A133" s="6" t="s">
+      <c r="A133" s="51" t="s">
         <v>712</v>
       </c>
       <c r="B133" s="4" t="s">
@@ -8336,7 +8342,7 @@
       <c r="M133" s="7"/>
     </row>
     <row r="134" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A134" s="6" t="s">
+      <c r="A134" s="50" t="s">
         <v>714</v>
       </c>
       <c r="B134" s="4" t="s">
@@ -8369,7 +8375,7 @@
       <c r="M134" s="7"/>
     </row>
     <row r="135" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A135" s="6" t="s">
+      <c r="A135" s="50" t="s">
         <v>713</v>
       </c>
       <c r="B135" s="4" t="s">
@@ -8402,7 +8408,7 @@
       <c r="M135" s="7"/>
     </row>
     <row r="136" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A136" s="6" t="s">
+      <c r="A136" s="50" t="s">
         <v>715</v>
       </c>
       <c r="B136" s="4" t="s">
@@ -8435,7 +8441,7 @@
       <c r="M136" s="7"/>
     </row>
     <row r="137" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A137" s="6" t="s">
+      <c r="A137" s="50" t="s">
         <v>716</v>
       </c>
       <c r="B137" s="4" t="s">
@@ -8470,7 +8476,7 @@
       <c r="M137" s="7"/>
     </row>
     <row r="138" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A138" s="6" t="s">
+      <c r="A138" s="50" t="s">
         <v>717</v>
       </c>
       <c r="B138" s="4" t="s">
@@ -8503,7 +8509,7 @@
       <c r="M138" s="7"/>
     </row>
     <row r="139" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A139" s="6" t="s">
+      <c r="A139" s="50" t="s">
         <v>718</v>
       </c>
       <c r="B139" s="4" t="s">
@@ -8536,7 +8542,7 @@
       <c r="M139" s="7"/>
     </row>
     <row r="140" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A140" s="6" t="s">
+      <c r="A140" s="51" t="s">
         <v>719</v>
       </c>
       <c r="B140" s="4" t="s">
@@ -8569,7 +8575,7 @@
       <c r="M140" s="7"/>
     </row>
     <row r="141" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A141" s="6" t="s">
+      <c r="A141" s="51" t="s">
         <v>720</v>
       </c>
       <c r="B141" s="4" t="s">
@@ -8602,7 +8608,7 @@
       <c r="M141" s="7"/>
     </row>
     <row r="142" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A142" s="6" t="s">
+      <c r="A142" s="51" t="s">
         <v>721</v>
       </c>
       <c r="B142" s="4" t="s">
@@ -8634,7 +8640,7 @@
       </c>
     </row>
     <row r="143" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A143" s="6" t="s">
+      <c r="A143" s="51" t="s">
         <v>722</v>
       </c>
       <c r="B143" s="4" t="s">
@@ -8666,7 +8672,7 @@
       </c>
     </row>
     <row r="144" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A144" s="6" t="s">
+      <c r="A144" s="50" t="s">
         <v>760</v>
       </c>
       <c r="B144" s="4" t="s">
@@ -8698,7 +8704,7 @@
       </c>
     </row>
     <row r="145" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A145" s="6" t="s">
+      <c r="A145" s="50" t="s">
         <v>762</v>
       </c>
       <c r="B145" s="4" t="s">
@@ -8730,7 +8736,7 @@
       </c>
     </row>
     <row r="146" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A146" s="6" t="s">
+      <c r="A146" s="50" t="s">
         <v>763</v>
       </c>
       <c r="B146" s="4" t="s">
@@ -8764,7 +8770,7 @@
       </c>
     </row>
     <row r="147" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A147" s="6" t="s">
+      <c r="A147" s="50" t="s">
         <v>347</v>
       </c>
       <c r="B147" s="4" t="s">
@@ -8796,7 +8802,7 @@
       </c>
     </row>
     <row r="148" spans="1:12" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A148" s="6" t="s">
+      <c r="A148" s="50" t="s">
         <v>764</v>
       </c>
       <c r="B148" s="4" t="s">
@@ -8828,7 +8834,7 @@
       </c>
     </row>
     <row r="149" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A149" s="6" t="s">
+      <c r="A149" s="50" t="s">
         <v>765</v>
       </c>
       <c r="B149" s="4" t="s">
@@ -8860,7 +8866,7 @@
       </c>
     </row>
     <row r="150" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A150" s="6" t="s">
+      <c r="A150" s="50" t="s">
         <v>766</v>
       </c>
       <c r="B150" s="4" t="s">
@@ -8890,7 +8896,7 @@
       </c>
     </row>
     <row r="151" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A151" s="6" t="s">
+      <c r="A151" s="50" t="s">
         <v>251</v>
       </c>
       <c r="B151" s="4" t="s">
@@ -8920,7 +8926,7 @@
       </c>
     </row>
     <row r="152" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A152" s="6" t="s">
+      <c r="A152" s="50" t="s">
         <v>767</v>
       </c>
       <c r="B152" s="4" t="s">
@@ -8952,7 +8958,7 @@
       </c>
     </row>
     <row r="153" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A153" s="6" t="s">
+      <c r="A153" s="50" t="s">
         <v>768</v>
       </c>
       <c r="B153" s="4" t="s">
@@ -12005,8 +12011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F102913-07D9-43F0-AADF-F13149DB4F36}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>